<commit_message>
Module 2. Task 2. Added results of using ADO.NET performance to exel-file.
</commit_message>
<xml_diff>
--- a/Module2/EF6_ChangeTracking.Perf.xlsx
+++ b/Module2/EF6_ChangeTracking.Perf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ChangeTracking = true</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Delete (seconds)</t>
+  </si>
+  <si>
+    <t>ADO.NET</t>
   </si>
 </sst>
 </file>
@@ -112,13 +115,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -145,13 +154,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -186,21 +201,57 @@
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -270,21 +321,57 @@
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -332,6 +419,126 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EFB1-4574-9E01-0208A1BBAA4A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADO.NET</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Insert (seconds)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Get (seconds)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Update (seconds)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Delete (seconds)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3663.1580300000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3525.27378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3821.5456399999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3634.1416599999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F42A-4B6D-AF92-4AE18984A2F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -357,9 +564,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -374,12 +581,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -389,7 +594,11 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -413,9 +622,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -431,12 +640,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -447,9 +654,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -490,9 +696,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -509,17 +714,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -582,62 +798,66 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -646,9 +866,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -667,14 +886,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -683,20 +894,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -705,13 +916,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -723,30 +934,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -762,21 +974,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -795,18 +1004,62 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -816,66 +1069,14 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:gridlineMajor>
   <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
@@ -885,14 +1086,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -904,14 +1104,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -923,14 +1123,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -939,14 +1138,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -954,7 +1152,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -967,11 +1165,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -979,14 +1185,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -998,12 +1204,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1019,7 +1232,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1028,9 +1241,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1046,14 +1258,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1062,20 +1273,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1087,12 +1295,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1395,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,6 +1660,23 @@
         <v>5452.0482000000002</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3663.1580300000001</v>
+      </c>
+      <c r="C4">
+        <v>3525.27378</v>
+      </c>
+      <c r="D4">
+        <v>3821.5456399999998</v>
+      </c>
+      <c r="E4">
+        <v>3634.1416599999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>